<commit_message>
Completed Changing the Margins, Scaling and Orientation
</commit_message>
<xml_diff>
--- a/09 - Printing an Excel Worksheet/MonthlyBudget.xlsx
+++ b/09 - Printing an Excel Worksheet/MonthlyBudget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/09 - Printing an Excel Worksheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BABA2F2A-F6A9-44B9-9684-9A9C0BF51CE2}"/>
+  <xr:revisionPtr revIDLastSave="170" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{123EA211-F34A-4315-BA53-E2FBEFDFFE06}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3512,15 +3512,15 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="912466" y="-128007"/>
-          <a:ext cx="2751602" cy="2751602"/>
+          <a:off x="711734" y="-93577"/>
+          <a:ext cx="2269925" cy="2269925"/>
         </a:xfrm>
         <a:prstGeom prst="circularArrow">
           <a:avLst>
             <a:gd name="adj1" fmla="val 5689"/>
             <a:gd name="adj2" fmla="val 340510"/>
-            <a:gd name="adj3" fmla="val 12595459"/>
-            <a:gd name="adj4" fmla="val 18147091"/>
+            <a:gd name="adj3" fmla="val 12698817"/>
+            <a:gd name="adj4" fmla="val 18075428"/>
             <a:gd name="adj5" fmla="val 5908"/>
           </a:avLst>
         </a:prstGeom>
@@ -3558,8 +3558,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1356424" y="259"/>
-          <a:ext cx="1863686" cy="931843"/>
+          <a:off x="1096476" y="50"/>
+          <a:ext cx="1500441" cy="750220"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -3601,12 +3601,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="60960" tIns="60960" rIns="60960" bIns="60960" numCol="1" spcCol="1270" anchor="t" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="49530" tIns="49530" rIns="49530" bIns="49530" numCol="1" spcCol="1270" anchor="t" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="711200">
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="577850">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3619,12 +3619,12 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-GB" sz="1600" kern="1200"/>
+            <a:rPr lang="en-GB" sz="1300" kern="1200"/>
             <a:t>Make Money</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr marL="114300" lvl="1" indent="-114300" algn="l" defTabSz="533400">
+          <a:pPr marL="57150" lvl="1" indent="-57150" algn="l" defTabSz="444500">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3637,12 +3637,12 @@
             <a:buChar char="•"/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-GB" sz="1200" kern="1200"/>
+            <a:rPr lang="en-GB" sz="1000" kern="1200"/>
             <a:t>Work</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr marL="114300" lvl="1" indent="-114300" algn="l" defTabSz="533400">
+          <a:pPr marL="57150" lvl="1" indent="-57150" algn="l" defTabSz="444500">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3655,14 +3655,14 @@
             <a:buChar char="•"/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-GB" sz="1200" kern="1200"/>
+            <a:rPr lang="en-GB" sz="1000" kern="1200"/>
             <a:t>Ask my Mum</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1401913" y="45748"/>
-        <a:ext cx="1772708" cy="840865"/>
+        <a:off x="1133099" y="36673"/>
+        <a:ext cx="1427195" cy="676974"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{27F9327D-FF5D-442E-8509-4F2240A0FD3E}">
@@ -3672,8 +3672,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2399293" y="1806562"/>
-          <a:ext cx="1863686" cy="931843"/>
+          <a:off x="1956788" y="1490155"/>
+          <a:ext cx="1500441" cy="750220"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -3715,12 +3715,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="60960" tIns="60960" rIns="60960" bIns="60960" numCol="1" spcCol="1270" anchor="t" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="49530" tIns="49530" rIns="49530" bIns="49530" numCol="1" spcCol="1270" anchor="t" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="711200">
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="577850">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3733,12 +3733,12 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-GB" sz="1600" kern="1200"/>
+            <a:rPr lang="en-GB" sz="1300" kern="1200"/>
             <a:t>Spend Money</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr marL="114300" lvl="1" indent="-114300" algn="l" defTabSz="533400">
+          <a:pPr marL="57150" lvl="1" indent="-57150" algn="l" defTabSz="444500">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3751,12 +3751,12 @@
             <a:buChar char="•"/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-GB" sz="1200" kern="1200"/>
+            <a:rPr lang="en-GB" sz="1000" kern="1200"/>
             <a:t>Bills</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr marL="114300" lvl="1" indent="-114300" algn="l" defTabSz="533400">
+          <a:pPr marL="57150" lvl="1" indent="-57150" algn="l" defTabSz="444500">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3769,14 +3769,14 @@
             <a:buChar char="•"/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-GB" sz="1200" kern="1200"/>
+            <a:rPr lang="en-GB" sz="1000" kern="1200"/>
             <a:t>Movie</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2444782" y="1852051"/>
-        <a:ext cx="1772708" cy="840865"/>
+        <a:off x="1993411" y="1526778"/>
+        <a:ext cx="1427195" cy="676974"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{925A5326-BFD1-4F4F-8989-7A005F690B8F}">
@@ -3786,8 +3786,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="313554" y="1806562"/>
-          <a:ext cx="1863686" cy="931843"/>
+          <a:off x="236164" y="1490155"/>
+          <a:ext cx="1500441" cy="750220"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -3829,12 +3829,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="60960" tIns="60960" rIns="60960" bIns="60960" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="49530" tIns="49530" rIns="49530" bIns="49530" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="711200">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3847,14 +3847,14 @@
             <a:buNone/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-GB" sz="1600" kern="1200"/>
+            <a:rPr lang="en-GB" sz="1300" kern="1200"/>
             <a:t>Track Money</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="359043" y="1852051"/>
-        <a:ext cx="1772708" cy="840865"/>
+        <a:off x="272787" y="1526778"/>
+        <a:ext cx="1427195" cy="676974"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -5444,15 +5444,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>307521</xdr:colOff>
+      <xdr:colOff>346400</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>111578</xdr:rowOff>
+      <xdr:rowOff>6867</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>103413</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>74385</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>199556</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>183241</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5479,16 +5479,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>216806</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>70755</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>160435</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>220951</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>524327</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>75291</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>467048</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>5052</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5866,10 +5866,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B2:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6169,10 +6172,11 @@
       <formula>250</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup fitToWidth="2" orientation="landscape" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="C13:E16 C11:F11" formulaRange="1"/>
   </ignoredErrors>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed Adding Header and Footer Content
</commit_message>
<xml_diff>
--- a/09 - Printing an Excel Worksheet/MonthlyBudget.xlsx
+++ b/09 - Printing an Excel Worksheet/MonthlyBudget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/09 - Printing an Excel Worksheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="170" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{123EA211-F34A-4315-BA53-E2FBEFDFFE06}"/>
+  <xr:revisionPtr revIDLastSave="171" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C99A31A-1FEF-4BD8-A98B-95A8D29B7BC6}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5871,8 +5871,8 @@
   </sheetPr>
   <dimension ref="B2:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6174,6 +6174,10 @@
   </conditionalFormatting>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup fitToWidth="2" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C2017 Monthly Budget&amp;RJames Cox</oddHeader>
+    <oddFooter>&amp;R&amp;P</oddFooter>
+  </headerFooter>
   <ignoredErrors>
     <ignoredError sqref="C13:E16 C11:F11" formulaRange="1"/>
   </ignoredErrors>

</xml_diff>